<commit_message>
small updates for the inputFormPage test
</commit_message>
<xml_diff>
--- a/seleniumeasy_exceldata_reader/src/main/resources/InputFormexcel.xlsx
+++ b/seleniumeasy_exceldata_reader/src/main/resources/InputFormexcel.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">My City</t>
   </si>
   <si>
-    <t xml:space="preserve">new mexico</t>
+    <t xml:space="preserve">New Mexico</t>
   </si>
   <si>
     <t xml:space="preserve">www.automation1.com</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Street Hello, No. 3</t>
   </si>
   <si>
-    <t xml:space="preserve">uttah</t>
+    <t xml:space="preserve">Uttah</t>
   </si>
   <si>
     <t xml:space="preserve">www.automation3.com</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Street Hello, No. 4</t>
   </si>
   <si>
-    <t xml:space="preserve">alabama</t>
+    <t xml:space="preserve">Alabama</t>
   </si>
   <si>
     <t xml:space="preserve">www.automation4.com</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">Street Hello, No. 5</t>
   </si>
   <si>
-    <t xml:space="preserve">hawaii</t>
+    <t xml:space="preserve">Hawaii</t>
   </si>
   <si>
     <t xml:space="preserve">www.automation5.com</t>
@@ -457,14 +457,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>